<commit_message>
UPDATE DIRECTORY KEY EMAIL
</commit_message>
<xml_diff>
--- a/ProcessFile/AIS_VERIFY_SPAM_SMS/Data/Config.xlsx
+++ b/ProcessFile/AIS_VERIFY_SPAM_SMS/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nampe\Documents\Uipath\AIS_PJ_NAME\ProcessFile\AIS_VERIFY_SPAM_SMS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BFCDE2-196F-4967-A3CD-4BC65E266B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0628FF2C-80FD-4F7B-911C-1B93628B048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -421,6 +421,12 @@
 &lt;/table&gt;
 $EMAIL_RESULT_TEMPLATE_FAILED
 &lt;h3 style="color: red"&gt; ***** นี่เป็นข้อความอัตโนมัติจากหุ่นยนต์ โปรดอย่าตอบกลับผ่าน E-mail นี้ ***** &lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>C:\Users\nampe\Documents\Uipath\AIS_PJ_NAME\MasterFile\EmailMaster.xlsx</t>
+  </si>
+  <si>
+    <t>EMAIL_MASTER</t>
   </si>
 </sst>
 </file>
@@ -804,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -940,7 +946,14 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4229,8 +4242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00022F7-58AE-485B-80A3-F9A3B1B706B4}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>